<commit_message>
commiting after implementation of data driven
</commit_message>
<xml_diff>
--- a/test_data/login_data.xlsx
+++ b/test_data/login_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pksin\PycharmProjects\SeleniumPythonProjects\saucedemo\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24169F2-E736-4AEC-AD2C-30DA40AAFDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF9F893-4DAD-44BF-9955-2A9B218A4971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -39,19 +39,28 @@
     <t>standard_user</t>
   </si>
   <si>
-    <t>visual_user</t>
-  </si>
-  <si>
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>incorrect_user</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>username_value</t>
+  </si>
+  <si>
+    <t>password_value</t>
+  </si>
+  <si>
+    <t>login_button</t>
+  </si>
+  <si>
+    <t>//input[@id ='user-name']</t>
+  </si>
+  <si>
+    <t>//input[@id ='password']</t>
+  </si>
+  <si>
+    <t>//input[@id ='login-button']</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -369,63 +378,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>